<commit_message>
auto:change the Clinical Health Library link
</commit_message>
<xml_diff>
--- a/config/forms/app/library.xlsx
+++ b/config/forms/app/library.xlsx
@@ -51,7 +51,7 @@
     <t>lib</t>
   </si>
   <si>
-    <t>[&lt;span style='background-color: #648af7; color:white; padding: 1em; text-decoration: none;border-radius: 8px; '&gt;Health Care Library&lt;/span&gt;](https://drive.google.com/drive/folders/1L0yg8qIyrcW4DJeVR1iKANfd2G5x37tp)</t>
+    <t>[&lt;span style='background-color: #648af7; color:white; padding: 1em; text-decoration: none;border-radius: 8px; '&gt;Health Care Library&lt;/span&gt;](https://drive.google.com/drive/folders/1dbNLvCfsU9Z1rhaMWu-4V0F2iG_U2Ysq)</t>
   </si>
   <si>
     <t>end group</t>
@@ -391,7 +391,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="108.5"/>
+    <col customWidth="1" min="3" max="3" width="180.75"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>